<commit_message>
Commit before adding alternative grid supply cost for ammonia plant
</commit_message>
<xml_diff>
--- a/Operating Guide/Discount Rate Converter.xlsx
+++ b/Operating Guide/Discount Rate Converter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioxfordnexus-my.sharepoint.com/personal/worc5561_ox_ac_uk/Documents/Coding/LCOH_Optimisation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioxfordnexus-my.sharepoint.com/personal/worc5561_ox_ac_uk/Documents/Coding/LCOA_Optimisation/Operating Guide/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="8_{EC819E99-A8F2-451E-9DF3-E71BA8A4B29F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BECA3C3A-8836-4FB6-B389-179AE0408F16}"/>
+  <xr:revisionPtr revIDLastSave="150" documentId="8_{EC819E99-A8F2-451E-9DF3-E71BA8A4B29F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4BACE8F-DFCB-4191-98E5-D2DA3914767A}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" activeTab="1" xr2:uid="{3526335E-7A46-450D-B03C-EEBC4F7D182F}"/>
+    <workbookView minimized="1" xWindow="2200" yWindow="2200" windowWidth="14400" windowHeight="8170" activeTab="1" xr2:uid="{3526335E-7A46-450D-B03C-EEBC4F7D182F}"/>
   </bookViews>
   <sheets>
     <sheet name="Simple" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>CAPEX</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>Outputs</t>
+  </si>
+  <si>
+    <t>O&amp;M (as frac)</t>
+  </si>
+  <si>
+    <t>O&amp;M (As value)</t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
 </sst>
 </file>
@@ -153,7 +162,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
@@ -161,6 +170,7 @@
     <xf numFmtId="2" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
@@ -469,7 +479,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -857,48 +867,52 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B062A89-8E27-4BF6-9DED-8650C74C1D43}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2">
-        <v>800000</v>
+        <v>600000</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2">
-        <v>0.1</v>
+        <v>8.7300000000000003E-2</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="6">
-        <f>SUM(C4:D34)</f>
-        <v>1017860.4052951788</v>
+        <f>SUM(C7:D37)</f>
+        <v>781271.33467567235</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="M1">
+        <v>13.41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2">
         <v>0.02</v>
@@ -908,558 +922,586 @@
         <v>4</v>
       </c>
       <c r="G2" s="4">
-        <f>SUM(B4:B34)</f>
-        <v>10.426914466988311</v>
+        <f>SUM(B7:B37)</f>
+        <v>10.1194284262181</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="M2">
+        <v>11.95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="5">
         <f>G1/G2</f>
-        <v>97618.562856512581</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4">
+        <v>77205.085284412082</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="7">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="C4" s="2">
-        <f>B1*B4</f>
-        <v>800000</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="C7" s="2">
+        <f>B1*B7</f>
+        <v>600000</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" ref="D7:D37" si="0">B7*($B$2*$C$7 + $B$3)</f>
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8">
         <v>1</v>
       </c>
-      <c r="B5">
-        <f t="shared" ref="B5:B20" si="0">B4/(1+$D$1)</f>
-        <v>0.90909090909090906</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2">
-        <f>$B$2*$C$4*B5</f>
-        <v>14545.454545454544</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <f t="shared" ref="A6:A34" si="1">A5+1</f>
+      <c r="B8">
+        <f t="shared" ref="B8:B37" si="1">IF(A8&lt;$B$4, B7/(1+$D$1), 0)</f>
+        <v>0.9197093718384991</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="0"/>
+        <v>11036.51246206199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <f t="shared" ref="A9:A37" si="2">A8+1</f>
         <v>2</v>
       </c>
-      <c r="B6" s="1">
-        <f t="shared" si="0"/>
-        <v>0.82644628099173545</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2">
-        <f>$B$2*$C$4*B6</f>
-        <v>13223.140495867767</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <f t="shared" si="1"/>
+      <c r="B9" s="1">
+        <f t="shared" si="1"/>
+        <v>0.84586532864756658</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="0"/>
+        <v>10150.383943770799</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="B7" s="1">
-        <f t="shared" si="0"/>
-        <v>0.75131480090157765</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2">
-        <f>$B$2*$C$4*B7</f>
-        <v>12021.036814425242</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <f t="shared" si="1"/>
+      <c r="B10" s="1">
+        <f t="shared" si="1"/>
+        <v>0.77795027007041906</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="0"/>
+        <v>9335.4032408450294</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="B8" s="1">
-        <f t="shared" si="0"/>
-        <v>0.68301345536507052</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2">
-        <f>$B$2*$C$4*B8</f>
-        <v>10928.215285841128</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <f t="shared" si="1"/>
+      <c r="B11" s="1">
+        <f t="shared" si="1"/>
+        <v>0.71548815420805578</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="0"/>
+        <v>8585.8578504966699</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="B9" s="1">
-        <f t="shared" si="0"/>
-        <v>0.62092132305915493</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2">
-        <f>$B$2*$C$4*B9</f>
-        <v>9934.7411689464789</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <f t="shared" si="1"/>
+      <c r="B12" s="1">
+        <f t="shared" si="1"/>
+        <v>0.6580411608645782</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" si="0"/>
+        <v>7896.4939303749388</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="B10" s="1">
-        <f t="shared" si="0"/>
-        <v>0.56447393005377711</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2">
-        <f>$B$2*$C$4*B10</f>
-        <v>9031.5828808604329</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <f t="shared" si="1"/>
+      <c r="B13" s="1">
+        <f t="shared" si="1"/>
+        <v>0.60520662270263792</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="0"/>
+        <v>7262.4794724316553</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="B11" s="1">
-        <f t="shared" si="0"/>
-        <v>0.51315811823070645</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0</v>
-      </c>
-      <c r="D11" s="2">
-        <f>$B$2*$C$4*B11</f>
-        <v>8210.5298916913034</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <f t="shared" si="1"/>
+      <c r="B14" s="1">
+        <f t="shared" si="1"/>
+        <v>0.55661420279834262</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="0"/>
+        <v>6679.3704335801112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="B12" s="1">
-        <f t="shared" si="0"/>
-        <v>0.46650738020973309</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0</v>
-      </c>
-      <c r="D12" s="2">
-        <f>$B$2*$C$4*B12</f>
-        <v>7464.1180833557291</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <f t="shared" si="1"/>
+      <c r="B15" s="1">
+        <f t="shared" si="1"/>
+        <v>0.51192329881205068</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="0"/>
+        <v>6143.0795857446083</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="B13" s="1">
-        <f t="shared" si="0"/>
-        <v>0.42409761837248461</v>
-      </c>
-      <c r="C13" s="2">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2">
-        <f>$B$2*$C$4*B13</f>
-        <v>6785.5618939597534</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="B14" s="1">
-        <f t="shared" si="0"/>
-        <v>0.38554328942953142</v>
-      </c>
-      <c r="C14" s="2">
-        <v>0</v>
-      </c>
-      <c r="D14" s="2">
-        <f>$B$2*$C$4*B14</f>
-        <v>6168.6926308725024</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="B15" s="1">
-        <f t="shared" si="0"/>
-        <v>0.35049389948139215</v>
-      </c>
-      <c r="C15" s="2">
-        <v>0</v>
-      </c>
-      <c r="D15" s="2">
-        <f>$B$2*$C$4*B15</f>
-        <v>5607.9023917022741</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
       <c r="B16" s="1">
-        <f t="shared" si="0"/>
-        <v>0.31863081771035645</v>
+        <f t="shared" si="1"/>
+        <v>0.47082065557992342</v>
       </c>
       <c r="C16" s="2">
         <v>0</v>
       </c>
       <c r="D16" s="2">
-        <f>$B$2*$C$4*B16</f>
-        <v>5098.093083365703</v>
+        <f t="shared" si="0"/>
+        <v>5649.8478669590813</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
-        <f t="shared" si="1"/>
-        <v>13</v>
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="B17" s="1">
-        <f t="shared" si="0"/>
-        <v>0.28966437973668768</v>
+        <f t="shared" si="1"/>
+        <v>0.43301816939200172</v>
       </c>
       <c r="C17" s="2">
         <v>0</v>
       </c>
       <c r="D17" s="2">
-        <f>$B$2*$C$4*B17</f>
-        <v>4634.6300757870031</v>
+        <f t="shared" si="0"/>
+        <v>5196.2180327040205</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
-        <f t="shared" si="1"/>
-        <v>14</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="B18" s="1">
-        <f t="shared" si="0"/>
-        <v>0.26333125430607968</v>
+        <f t="shared" si="1"/>
+        <v>0.3982508685661747</v>
       </c>
       <c r="C18" s="2">
         <v>0</v>
       </c>
       <c r="D18" s="2">
-        <f>$B$2*$C$4*B18</f>
-        <v>4213.3000688972752</v>
+        <f t="shared" si="0"/>
+        <v>4779.0104227940965</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
-        <f t="shared" si="1"/>
-        <v>15</v>
+        <f t="shared" si="2"/>
+        <v>12</v>
       </c>
       <c r="B19" s="1">
-        <f t="shared" si="0"/>
-        <v>0.23939204936916333</v>
+        <f t="shared" si="1"/>
+        <v>0.36627505616313322</v>
       </c>
       <c r="C19" s="2">
-        <f>C4*0.35*B19</f>
-        <v>67029.773823365729</v>
+        <v>0</v>
       </c>
       <c r="D19" s="2">
-        <f>$B$2*$C$4*B19</f>
-        <v>3830.2727899066135</v>
+        <f t="shared" si="0"/>
+        <v>4395.3006739575985</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
-        <f t="shared" si="1"/>
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>13</v>
       </c>
       <c r="B20" s="1">
-        <f t="shared" si="0"/>
-        <v>0.21762913579014848</v>
+        <f t="shared" si="1"/>
+        <v>0.33686660182390621</v>
       </c>
       <c r="C20" s="2">
         <v>0</v>
       </c>
       <c r="D20" s="2">
-        <f>$B$2*$C$4*B20</f>
-        <v>3482.0661726423755</v>
+        <f t="shared" si="0"/>
+        <v>4042.3992218868743</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
-        <f t="shared" si="1"/>
-        <v>17</v>
+        <f t="shared" si="2"/>
+        <v>14</v>
       </c>
       <c r="B21" s="1">
-        <f t="shared" ref="B21:B34" si="2">B20/(1+$D$1)</f>
-        <v>0.19784466890013497</v>
+        <f t="shared" si="1"/>
+        <v>0.30981937075683458</v>
       </c>
       <c r="C21" s="2">
         <v>0</v>
       </c>
       <c r="D21" s="2">
-        <f>$B$2*$C$4*B21</f>
-        <v>3165.5147024021594</v>
+        <f t="shared" si="0"/>
+        <v>3717.832449082015</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
-        <f t="shared" si="1"/>
-        <v>18</v>
+        <f t="shared" si="2"/>
+        <v>15</v>
       </c>
       <c r="B22" s="1">
-        <f t="shared" si="2"/>
-        <v>0.17985878990921358</v>
+        <f t="shared" si="1"/>
+        <v>0.28494377886216737</v>
       </c>
       <c r="C22" s="2">
-        <v>0</v>
+        <f>C7*0.35*B22</f>
+        <v>59838.193561055152</v>
       </c>
       <c r="D22" s="2">
-        <f>$B$2*$C$4*B22</f>
-        <v>2877.7406385474173</v>
+        <f t="shared" si="0"/>
+        <v>3419.3253463460087</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
-        <f t="shared" si="1"/>
-        <v>19</v>
+        <f t="shared" si="2"/>
+        <v>16</v>
       </c>
       <c r="B23" s="1">
-        <f t="shared" si="2"/>
-        <v>0.16350799082655779</v>
+        <f t="shared" si="1"/>
+        <v>0.26206546386661217</v>
       </c>
       <c r="C23" s="2">
         <v>0</v>
       </c>
       <c r="D23" s="2">
-        <f>$B$2*$C$4*B23</f>
-        <v>2616.1278532249244</v>
+        <f t="shared" si="0"/>
+        <v>3144.785566399346</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
-        <f t="shared" si="1"/>
-        <v>20</v>
+        <f t="shared" si="2"/>
+        <v>17</v>
       </c>
       <c r="B24" s="1">
-        <f t="shared" si="2"/>
-        <v>0.14864362802414344</v>
+        <f t="shared" si="1"/>
+        <v>0.24102406315332675</v>
       </c>
       <c r="C24" s="2">
         <v>0</v>
       </c>
       <c r="D24" s="2">
-        <f>$B$2*$C$4*B24</f>
-        <v>2378.2980483862948</v>
+        <f t="shared" si="0"/>
+        <v>2892.2887578399209</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
-        <f t="shared" si="1"/>
-        <v>21</v>
+        <f t="shared" si="2"/>
+        <v>18</v>
       </c>
       <c r="B25" s="1">
-        <f t="shared" si="2"/>
-        <v>0.13513057093103947</v>
+        <f t="shared" si="1"/>
+        <v>0.22167208972070887</v>
       </c>
       <c r="C25" s="2">
         <v>0</v>
       </c>
       <c r="D25" s="2">
-        <f>$B$2*$C$4*B25</f>
-        <v>2162.0891348966315</v>
+        <f t="shared" si="0"/>
+        <v>2660.0650766485064</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
-        <f t="shared" si="1"/>
-        <v>22</v>
+        <f t="shared" si="2"/>
+        <v>19</v>
       </c>
       <c r="B26" s="1">
-        <f t="shared" si="2"/>
-        <v>0.12284597357367223</v>
+        <f t="shared" si="1"/>
+        <v>0.20387389839116057</v>
       </c>
       <c r="C26" s="2">
         <v>0</v>
       </c>
       <c r="D26" s="2">
-        <f>$B$2*$C$4*B26</f>
-        <v>1965.5355771787556</v>
+        <f t="shared" si="0"/>
+        <v>2446.4867806939269</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
-        <f t="shared" si="1"/>
-        <v>23</v>
+        <f t="shared" si="2"/>
+        <v>20</v>
       </c>
       <c r="B27" s="1">
-        <f t="shared" si="2"/>
-        <v>0.11167815779424747</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="C27" s="2">
         <v>0</v>
       </c>
       <c r="D27" s="2">
-        <f>$B$2*$C$4*B27</f>
-        <v>1786.8505247079595</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
-        <f t="shared" si="1"/>
-        <v>24</v>
+        <f t="shared" si="2"/>
+        <v>21</v>
       </c>
       <c r="B28" s="1">
-        <f t="shared" si="2"/>
-        <v>0.10152559799477043</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="C28" s="2">
         <v>0</v>
       </c>
       <c r="D28" s="2">
-        <f>$B$2*$C$4*B28</f>
-        <v>1624.4095679163268</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
-        <f t="shared" si="1"/>
-        <v>25</v>
+        <f t="shared" si="2"/>
+        <v>22</v>
       </c>
       <c r="B29" s="1">
-        <f t="shared" si="2"/>
-        <v>9.229599817706402E-2</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="C29" s="2">
         <v>0</v>
       </c>
       <c r="D29" s="2">
-        <f>$B$2*$C$4*B29</f>
-        <v>1476.7359708330243</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
-        <f t="shared" si="1"/>
-        <v>26</v>
+        <f t="shared" si="2"/>
+        <v>23</v>
       </c>
       <c r="B30" s="1">
-        <f t="shared" si="2"/>
-        <v>8.3905452888240015E-2</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="C30" s="2">
         <v>0</v>
       </c>
       <c r="D30" s="2">
-        <f>$B$2*$C$4*B30</f>
-        <v>1342.4872462118403</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31">
-        <f t="shared" si="1"/>
-        <v>27</v>
+        <f t="shared" si="2"/>
+        <v>24</v>
       </c>
       <c r="B31" s="1">
-        <f t="shared" si="2"/>
-        <v>7.6277684443854549E-2</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="C31" s="2">
         <v>0</v>
       </c>
       <c r="D31" s="2">
-        <f>$B$2*$C$4*B31</f>
-        <v>1220.4429511016729</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32">
-        <f t="shared" si="1"/>
-        <v>28</v>
+        <f t="shared" si="2"/>
+        <v>25</v>
       </c>
       <c r="B32" s="1">
-        <f t="shared" si="2"/>
-        <v>6.9343349494413217E-2</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="C32" s="2">
         <v>0</v>
       </c>
       <c r="D32" s="2">
-        <f>$B$2*$C$4*B32</f>
-        <v>1109.4935919106115</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33">
-        <f t="shared" si="1"/>
-        <v>29</v>
+        <f t="shared" si="2"/>
+        <v>26</v>
       </c>
       <c r="B33" s="1">
-        <f t="shared" si="2"/>
-        <v>6.3039408631284738E-2</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="C33" s="2">
         <v>0</v>
       </c>
       <c r="D33" s="2">
-        <f>$B$2*$C$4*B33</f>
-        <v>1008.6305381005558</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="B34" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0</v>
+      </c>
+      <c r="D34" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="B35" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0</v>
+      </c>
+      <c r="D35" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="B36" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0</v>
+      </c>
+      <c r="D36" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="B34" s="1">
-        <f t="shared" si="2"/>
-        <v>5.7308553301167936E-2</v>
-      </c>
-      <c r="C34" s="2">
-        <v>0</v>
-      </c>
-      <c r="D34" s="2">
-        <f>$B$2*$C$4*B34</f>
-        <v>916.93685281868693</v>
+      <c r="B37" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0</v>
+      </c>
+      <c r="D37" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>